<commit_message>
Adición tabla sql personalserviciomilitarobligatorio.sql y cambio emcabezado MDN
</commit_message>
<xml_diff>
--- a/DOCUMENTOS EXCEL/MDN.xlsx
+++ b/DOCUMENTOS EXCEL/MDN.xlsx
@@ -8,25 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\desarrollomarlon\DOCUMENTOS EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C99843-0B80-403C-BE6B-E4DDBBD2059C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00677484-C104-4489-A3B5-E310BE15AAF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Militares MDN Activos-4.2" sheetId="21" r:id="rId1"/>
     <sheet name="Res MilitActv Contingencias 4.3" sheetId="8" r:id="rId2"/>
     <sheet name="ResPerPSMOyALMActvs4.4YContg4.5" sheetId="15" r:id="rId3"/>
     <sheet name="RsFutOfiSubSlpIMPperSMOByALM4.6" sheetId="36" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="37" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'ResPerPSMOyALMActvs4.4YContg4.5'!$B$1:$O$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="72">
   <si>
     <t>TOTAL</t>
   </si>
@@ -234,6 +236,15 @@
   </si>
   <si>
     <t>FUERZA AÉREA- SUBOFICIAL - 15/20</t>
+  </si>
+  <si>
+    <t>INSERT INTO personalserviciomilitarobligatorioyalumnos VALUES(</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>);</t>
   </si>
 </sst>
 </file>
@@ -248,9 +259,9 @@
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;\ * #,##0.00_);_(&quot;$&quot;\ * \(#,##0.00\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="#,##0.00000"/>
-    <numFmt numFmtId="169" formatCode="#,##0;[Red]#,##0"/>
-    <numFmt numFmtId="170" formatCode="_-[$$-240A]\ * #,##0.00_-;\-[$$-240A]\ * #,##0.00_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="168" formatCode="#,##0;[Red]#,##0"/>
+    <numFmt numFmtId="169" formatCode="_-[$$-240A]\ * #,##0.00_-;\-[$$-240A]\ * #,##0.00_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -406,7 +417,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -749,6 +760,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -758,7 +780,7 @@
     <xf numFmtId="165" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
@@ -781,7 +803,7 @@
     <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -889,13 +911,13 @@
     <xf numFmtId="3" fontId="8" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -913,13 +935,13 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -983,13 +1005,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="28" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1047,6 +1069,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2996,8 +3037,8 @@
   </sheetPr>
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G2" zoomScaleNormal="100" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="95" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3048,14 +3089,14 @@
       <c r="G2" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="108"/>
+      <c r="M2" s="108"/>
+      <c r="N2" s="108"/>
+      <c r="O2" s="108"/>
     </row>
     <row r="3" spans="1:16" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
@@ -3064,21 +3105,21 @@
       <c r="D3" s="101"/>
       <c r="E3" s="101"/>
       <c r="F3" s="69"/>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="68"/>
-      <c r="I3" s="97" t="s">
+      <c r="H3" s="106"/>
+      <c r="I3" s="107" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="97" t="s">
+      <c r="K3" s="110"/>
+      <c r="L3" s="106"/>
+      <c r="M3" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
+      <c r="N3" s="111"/>
+      <c r="O3" s="107"/>
     </row>
     <row r="4" spans="1:16" s="19" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
@@ -3096,20 +3137,20 @@
       <c r="G4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="6" t="s">
+      <c r="H4" s="109"/>
+      <c r="I4" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="68"/>
-      <c r="K4" s="6" t="s">
+      <c r="J4" s="109"/>
+      <c r="K4" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="L4" s="68"/>
-      <c r="M4" s="6" t="s">
+      <c r="L4" s="109"/>
+      <c r="M4" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="68"/>
-      <c r="O4" s="6" t="s">
+      <c r="N4" s="109"/>
+      <c r="O4" s="109" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3185,39 +3226,39 @@
         <v>1327258.6402230498</v>
       </c>
       <c r="G6" s="48">
-        <f t="shared" ref="G6:G11" si="0">+F6*P6</f>
+        <f>+F6*P6</f>
         <v>106500363648.65271</v>
       </c>
       <c r="H6" s="48">
         <v>414.89213015746662</v>
       </c>
       <c r="I6" s="48">
-        <f t="shared" ref="I6:I11" si="1">+H6*P6</f>
+        <f t="shared" ref="I6:I11" si="0">+H6*P6</f>
         <v>33291297.865884475</v>
       </c>
       <c r="J6" s="48">
         <v>1111073.5645834447</v>
       </c>
       <c r="K6" s="48">
-        <f t="shared" ref="K6:K11" si="2">+J6*P6</f>
+        <f t="shared" ref="K6:K11" si="1">+J6*P6</f>
         <v>89153489065.745331</v>
       </c>
       <c r="L6" s="48">
         <v>174.1637201098149</v>
       </c>
       <c r="M6" s="48">
-        <f t="shared" ref="M6:M11" si="3">+L6*P6</f>
+        <f t="shared" ref="M6:M11" si="2">+L6*P6</f>
         <v>13975045.227793979</v>
       </c>
       <c r="N6" s="48">
         <v>958896.08368714771</v>
       </c>
       <c r="O6" s="48">
-        <f t="shared" ref="O6:O11" si="4">+N6*P6</f>
+        <f t="shared" ref="O6:O11" si="3">+N6*P6</f>
         <v>76942638396.980499</v>
       </c>
       <c r="P6" s="81">
-        <f t="shared" ref="P6:P11" si="5">+SUM(C6:E6)</f>
+        <f>+SUM(C6:E6)</f>
         <v>80240.851647991542</v>
       </c>
     </row>
@@ -3239,39 +3280,39 @@
         <v>1296511.5726366274</v>
       </c>
       <c r="G7" s="48">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G6:G11" si="4">+F7*P7</f>
         <v>1895097798.2326298</v>
       </c>
       <c r="H7" s="48">
         <v>260.56501888120545</v>
       </c>
       <c r="I7" s="48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>380865.24177645118</v>
       </c>
       <c r="J7" s="48">
         <v>1085846.2448595848</v>
       </c>
       <c r="K7" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1587170428.1572986</v>
       </c>
       <c r="L7" s="48">
         <v>98.963013766702005</v>
       </c>
       <c r="M7" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>144653.23214535273</v>
       </c>
       <c r="N7" s="48">
         <v>937124.00769125985</v>
       </c>
       <c r="O7" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1369784644.5250256</v>
       </c>
       <c r="P7" s="81">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="P6:P11" si="5">+SUM(C7:E7)</f>
         <v>1461.689843908372</v>
       </c>
     </row>
@@ -3293,35 +3334,35 @@
         <v>0</v>
       </c>
       <c r="G8" s="48">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="48">
+        <v>0</v>
+      </c>
+      <c r="I8" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="48">
+      <c r="J8" s="48">
         <v>0</v>
       </c>
-      <c r="I8" s="48">
+      <c r="K8" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J8" s="48">
+      <c r="L8" s="48">
         <v>0</v>
       </c>
-      <c r="K8" s="48">
+      <c r="M8" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L8" s="48">
-        <v>0</v>
-      </c>
-      <c r="M8" s="48">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="N8" s="48">
         <v>0</v>
       </c>
       <c r="O8" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P8" s="81">
@@ -3347,35 +3388,35 @@
         <v>1182163.3059787424</v>
       </c>
       <c r="G9" s="48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>6286813405.9095926</v>
       </c>
       <c r="H9" s="48">
         <v>609.60546118951868</v>
       </c>
       <c r="I9" s="48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3241917.3952865703</v>
       </c>
       <c r="J9" s="48">
         <v>28626.412798941259</v>
       </c>
       <c r="K9" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>152236932.78018394</v>
       </c>
       <c r="L9" s="48">
         <v>480.82470986366383</v>
       </c>
       <c r="M9" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2557053.8491386981</v>
       </c>
       <c r="N9" s="48">
         <v>29713.732623592998</v>
       </c>
       <c r="O9" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>158019363.02104843</v>
       </c>
       <c r="P9" s="81">
@@ -3401,35 +3442,35 @@
         <v>2319920.3393907701</v>
       </c>
       <c r="G10" s="48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>6395298722.5882225</v>
       </c>
       <c r="H10" s="48">
         <v>1774.1870198665804</v>
       </c>
       <c r="I10" s="48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4890881.7208633199</v>
       </c>
       <c r="J10" s="48">
         <v>56177.515278379855</v>
       </c>
       <c r="K10" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>154863934.59197432</v>
       </c>
       <c r="L10" s="48">
         <v>1399.385030599881</v>
       </c>
       <c r="M10" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3857669.2253815522</v>
       </c>
       <c r="N10" s="48">
         <v>58311.311229796782</v>
       </c>
       <c r="O10" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>160746146.27427036</v>
       </c>
       <c r="P10" s="81">
@@ -3455,35 +3496,35 @@
         <v>745673.42383563949</v>
       </c>
       <c r="G11" s="48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>202265964.7687794</v>
       </c>
       <c r="H11" s="48">
         <v>0</v>
       </c>
       <c r="I11" s="48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J11" s="48">
         <v>22487.265521533878</v>
       </c>
       <c r="K11" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6099732.5509180473</v>
       </c>
       <c r="L11" s="48">
         <v>0</v>
       </c>
       <c r="M11" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N11" s="48">
         <v>23341.401549789804</v>
       </c>
       <c r="O11" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>6331419.2951100171</v>
       </c>
       <c r="P11" s="81">
@@ -4077,7 +4118,7 @@
   </sheetPr>
   <dimension ref="B4:D13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="89" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="89" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -4188,4 +4229,500 @@
   <pageMargins left="0.7" right="0.7" top="1.19" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="87" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE92FDB8-2C1A-4232-B05D-2DD77F55330A}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:U7"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:U7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="64"/>
+    <col min="3" max="3" width="11.42578125" style="64"/>
+    <col min="4" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="64">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="64">
+        <v>2020</v>
+      </c>
+      <c r="D1" s="105">
+        <v>6561.666869383067</v>
+      </c>
+      <c r="E1" s="105">
+        <v>4092.7828872584482</v>
+      </c>
+      <c r="F1" s="105">
+        <v>2235.0087514585762</v>
+      </c>
+      <c r="G1" s="105">
+        <v>1573096.7815331558</v>
+      </c>
+      <c r="H1" s="105">
+        <v>20276365694.797405</v>
+      </c>
+      <c r="I1" s="105">
+        <v>16624.199328198367</v>
+      </c>
+      <c r="J1" s="105">
+        <v>214276927.47119826</v>
+      </c>
+      <c r="K1" s="105">
+        <v>1313078.7017581831</v>
+      </c>
+      <c r="L1" s="105">
+        <v>16924873444.182035</v>
+      </c>
+      <c r="M1" s="105">
+        <v>7226.3106341511311</v>
+      </c>
+      <c r="N1" s="105">
+        <v>93143231.08553347</v>
+      </c>
+      <c r="O1" s="105">
+        <v>1133233.716312007</v>
+      </c>
+      <c r="P1" s="105">
+        <v>14606768966.383684</v>
+      </c>
+      <c r="Q1" s="105">
+        <v>12889.458508100091</v>
+      </c>
+      <c r="R1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T1" t="str">
+        <f>A1&amp;R1&amp;B1&amp;R1&amp;C1&amp;R1&amp;D1&amp;R1&amp;E1&amp;R1&amp;F1&amp;R1&amp;G1&amp;R1&amp;H1&amp;R1&amp;I1&amp;R1&amp;J1&amp;R1&amp;K1&amp;R1&amp;L1&amp;R1&amp;M1&amp;R1&amp;N1&amp;R1&amp;O1&amp;R1&amp;P1&amp;R1&amp;Q1&amp;R1</f>
+        <v>1;1;2020;6561,66686938307;4092,78288725845;2235,00875145858;1573096,78153316;20276365694,7974;16624,1993281984;214276927,471198;1313078,70175818;16924873444,182;7226,31063415113;93143231,0855335;1133233,71631201;14606768966,3837;12889,4585081001;</v>
+      </c>
+      <c r="U1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="64">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="64">
+        <v>2020</v>
+      </c>
+      <c r="D2" s="105">
+        <v>76211.643286708568</v>
+      </c>
+      <c r="E2" s="105">
+        <v>3069.2171127415518</v>
+      </c>
+      <c r="F2" s="105">
+        <v>959.9912485414236</v>
+      </c>
+      <c r="G2" s="105">
+        <v>1327258.6402230498</v>
+      </c>
+      <c r="H2" s="105">
+        <v>106500363648.65271</v>
+      </c>
+      <c r="I2" s="105">
+        <v>414.89213015746662</v>
+      </c>
+      <c r="J2" s="105">
+        <v>33291297.865884475</v>
+      </c>
+      <c r="K2" s="105">
+        <v>1111073.5645834447</v>
+      </c>
+      <c r="L2" s="105">
+        <v>89153489065.745331</v>
+      </c>
+      <c r="M2" s="105">
+        <v>174.1637201098149</v>
+      </c>
+      <c r="N2" s="105">
+        <v>13975045.227793979</v>
+      </c>
+      <c r="O2" s="105">
+        <v>958896.08368714771</v>
+      </c>
+      <c r="P2" s="105">
+        <v>76942638396.980499</v>
+      </c>
+      <c r="Q2" s="105">
+        <v>80240.851647991542</v>
+      </c>
+      <c r="R2" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="S2" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="T2" s="64" t="str">
+        <f t="shared" ref="T2:T7" si="0">A2&amp;R2&amp;B2&amp;R2&amp;C2&amp;R2&amp;D2&amp;R2&amp;E2&amp;R2&amp;F2&amp;R2&amp;G2&amp;R2&amp;H2&amp;R2&amp;I2&amp;R2&amp;J2&amp;R2&amp;K2&amp;R2&amp;L2&amp;R2&amp;M2&amp;R2&amp;N2&amp;R2&amp;O2&amp;R2&amp;P2&amp;R2&amp;Q2&amp;R2</f>
+        <v>2;2;2020;76211,6432867086;3069,21711274155;959,991248541424;1327258,64022305;106500363648,653;414,892130157467;33291297,8658845;1111073,56458344;89153489065,7453;174,163720109815;13975045,227794;958896,083687148;76942638396,9805;80240,8516479915;</v>
+      </c>
+      <c r="U2" s="64" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="64">
+        <v>3</v>
+      </c>
+      <c r="B3" s="64">
+        <v>3</v>
+      </c>
+      <c r="C3" s="64">
+        <v>2020</v>
+      </c>
+      <c r="D3" s="105">
+        <v>1461.689843908372</v>
+      </c>
+      <c r="E3" s="105">
+        <v>0</v>
+      </c>
+      <c r="F3" s="105">
+        <v>0</v>
+      </c>
+      <c r="G3" s="105">
+        <v>1296511.5726366274</v>
+      </c>
+      <c r="H3" s="105">
+        <v>1895097798.2326298</v>
+      </c>
+      <c r="I3" s="105">
+        <v>260.56501888120545</v>
+      </c>
+      <c r="J3" s="105">
+        <v>380865.24177645118</v>
+      </c>
+      <c r="K3" s="105">
+        <v>1085846.2448595848</v>
+      </c>
+      <c r="L3" s="105">
+        <v>1587170428.1572986</v>
+      </c>
+      <c r="M3" s="105">
+        <v>98.963013766702005</v>
+      </c>
+      <c r="N3" s="105">
+        <v>144653.23214535273</v>
+      </c>
+      <c r="O3" s="105">
+        <v>937124.00769125985</v>
+      </c>
+      <c r="P3" s="105">
+        <v>1369784644.5250256</v>
+      </c>
+      <c r="Q3" s="105">
+        <v>1461.689843908372</v>
+      </c>
+      <c r="R3" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="T3" s="64" t="str">
+        <f t="shared" si="0"/>
+        <v>3;3;2020;1461,68984390837;0;0;1296511,57263663;1895097798,23263;260,565018881205;380865,241776451;1085846,24485958;1587170428,1573;98,963013766702;144653,232145353;937124,00769126;1369784644,52503;1461,68984390837;</v>
+      </c>
+      <c r="U3" s="64" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="64">
+        <v>4</v>
+      </c>
+      <c r="B4" s="64">
+        <v>4</v>
+      </c>
+      <c r="C4" s="64">
+        <v>2020</v>
+      </c>
+      <c r="D4" s="105">
+        <v>0</v>
+      </c>
+      <c r="E4" s="105">
+        <v>0</v>
+      </c>
+      <c r="F4" s="105">
+        <v>0</v>
+      </c>
+      <c r="G4" s="105">
+        <v>0</v>
+      </c>
+      <c r="H4" s="105">
+        <v>0</v>
+      </c>
+      <c r="I4" s="105">
+        <v>0</v>
+      </c>
+      <c r="J4" s="105">
+        <v>0</v>
+      </c>
+      <c r="K4" s="105">
+        <v>0</v>
+      </c>
+      <c r="L4" s="105">
+        <v>0</v>
+      </c>
+      <c r="M4" s="105">
+        <v>0</v>
+      </c>
+      <c r="N4" s="105">
+        <v>0</v>
+      </c>
+      <c r="O4" s="105">
+        <v>0</v>
+      </c>
+      <c r="P4" s="105">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="105">
+        <v>0</v>
+      </c>
+      <c r="R4" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="S4" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="T4" s="64" t="str">
+        <f t="shared" si="0"/>
+        <v>4;4;2020;0;0;0;0;0;0;0;0;0;0;0;0;0;0;</v>
+      </c>
+      <c r="U4" s="64" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="64">
+        <v>5</v>
+      </c>
+      <c r="B5" s="64">
+        <v>5</v>
+      </c>
+      <c r="C5" s="64">
+        <v>2020</v>
+      </c>
+      <c r="D5" s="105">
+        <v>4390.4773557921499</v>
+      </c>
+      <c r="E5" s="105">
+        <v>640.01465201465203</v>
+      </c>
+      <c r="F5" s="105">
+        <v>287.56631299734744</v>
+      </c>
+      <c r="G5" s="105">
+        <v>1182163.3059787424</v>
+      </c>
+      <c r="H5" s="105">
+        <v>6286813405.9095926</v>
+      </c>
+      <c r="I5" s="105">
+        <v>609.60546118951868</v>
+      </c>
+      <c r="J5" s="105">
+        <v>3241917.3952865703</v>
+      </c>
+      <c r="K5" s="105">
+        <v>28626.412798941259</v>
+      </c>
+      <c r="L5" s="105">
+        <v>152236932.78018394</v>
+      </c>
+      <c r="M5" s="105">
+        <v>480.82470986366383</v>
+      </c>
+      <c r="N5" s="105">
+        <v>2557053.8491386981</v>
+      </c>
+      <c r="O5" s="105">
+        <v>29713.732623592998</v>
+      </c>
+      <c r="P5" s="105">
+        <v>158019363.02104843</v>
+      </c>
+      <c r="Q5" s="105">
+        <v>5318.0583208041489</v>
+      </c>
+      <c r="R5" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="S5" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="T5" s="64" t="str">
+        <f t="shared" si="0"/>
+        <v>5;5;2020;4390,47735579215;640,014652014652;287,566312997347;1182163,30597874;6286813405,90959;609,605461189519;3241917,39528657;28626,4127989413;152236932,780184;480,824709863664;2557053,8491387;29713,732623593;158019363,021048;5318,05832080415;</v>
+      </c>
+      <c r="U5" s="64" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="64">
+        <v>6</v>
+      </c>
+      <c r="B6" s="64">
+        <v>6</v>
+      </c>
+      <c r="C6" s="64">
+        <v>2020</v>
+      </c>
+      <c r="D6" s="105">
+        <v>1768.5226442078499</v>
+      </c>
+      <c r="E6" s="105">
+        <v>540.73260073260076</v>
+      </c>
+      <c r="F6" s="105">
+        <v>447.4336870026525</v>
+      </c>
+      <c r="G6" s="105">
+        <v>2319920.3393907701</v>
+      </c>
+      <c r="H6" s="105">
+        <v>6395298722.5882225</v>
+      </c>
+      <c r="I6" s="105">
+        <v>1774.1870198665804</v>
+      </c>
+      <c r="J6" s="105">
+        <v>4890881.7208633199</v>
+      </c>
+      <c r="K6" s="105">
+        <v>56177.515278379855</v>
+      </c>
+      <c r="L6" s="105">
+        <v>154863934.59197432</v>
+      </c>
+      <c r="M6" s="105">
+        <v>1399.385030599881</v>
+      </c>
+      <c r="N6" s="105">
+        <v>3857669.2253815522</v>
+      </c>
+      <c r="O6" s="105">
+        <v>58311.311229796782</v>
+      </c>
+      <c r="P6" s="105">
+        <v>160746146.27427036</v>
+      </c>
+      <c r="Q6" s="105">
+        <v>2756.6889319431029</v>
+      </c>
+      <c r="R6" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="S6" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="T6" s="64" t="str">
+        <f t="shared" si="0"/>
+        <v>6;6;2020;1768,52264420785;540,732600732601;447,433687002653;2319920,33939077;6395298722,58822;1774,18701986658;4890881,72086332;56177,5152783799;154863934,591974;1399,38503059988;3857669,22538155;58311,3112297968;160746146,27427;2756,6889319431;</v>
+      </c>
+      <c r="U6" s="64" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="64">
+        <v>7</v>
+      </c>
+      <c r="B7" s="64">
+        <v>7</v>
+      </c>
+      <c r="C7" s="64">
+        <v>2020</v>
+      </c>
+      <c r="D7" s="105">
+        <v>0</v>
+      </c>
+      <c r="E7" s="105">
+        <v>271.25274725274727</v>
+      </c>
+      <c r="F7" s="105">
+        <v>0</v>
+      </c>
+      <c r="G7" s="105">
+        <v>745673.42383563949</v>
+      </c>
+      <c r="H7" s="105">
+        <v>202265964.7687794</v>
+      </c>
+      <c r="I7" s="105">
+        <v>0</v>
+      </c>
+      <c r="J7" s="105">
+        <v>0</v>
+      </c>
+      <c r="K7" s="105">
+        <v>22487.265521533878</v>
+      </c>
+      <c r="L7" s="105">
+        <v>6099732.5509180473</v>
+      </c>
+      <c r="M7" s="105">
+        <v>0</v>
+      </c>
+      <c r="N7" s="105">
+        <v>0</v>
+      </c>
+      <c r="O7" s="105">
+        <v>23341.401549789804</v>
+      </c>
+      <c r="P7" s="105">
+        <v>6331419.2951100171</v>
+      </c>
+      <c r="Q7" s="105">
+        <v>271.25274725274727</v>
+      </c>
+      <c r="R7" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="S7" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="T7" s="64" t="str">
+        <f t="shared" si="0"/>
+        <v>7;7;2020;0;271,252747252747;0;745673,423835639;202265964,768779;0;0;22487,2655215339;6099732,55091805;0;0;23341,4015497898;6331419,29511002;271,252747252747;</v>
+      </c>
+      <c r="U7" s="64" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>